<commit_message>
updated dependencies mainly because drf_yasg no longer installs cleanly. autocomplete_light also had some breaking updates and I added the lastest (last?) version of jquery
</commit_message>
<xml_diff>
--- a/static/bulk_template.xlsx
+++ b/static/bulk_template.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PlasmidBatch" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Plasmid" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Plasmid" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PlasmidBatch" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Strain" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Fermentation" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
@@ -416,6 +416,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Batches</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -448,47 +489,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Parent</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>responsible</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Batches</t>
         </is>
       </c>
     </row>

</xml_diff>